<commit_message>
day 1 session 1
</commit_message>
<xml_diff>
--- a/GET July 2021 - Training Plan with Hourly breakup.xlsx
+++ b/GET July 2021 - Training Plan with Hourly breakup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
   <si>
     <t xml:space="preserve">Java training </t>
   </si>
@@ -54,7 +54,10 @@
 Java Archite-cture, JDK,JRE,Array, Loops, dry run, examples and practice</t>
   </si>
   <si>
-    <t xml:space="preserve">17th July</t>
+    <t xml:space="preserve">19th July 20th July</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2+1/2</t>
   </si>
   <si>
     <t xml:space="preserve">8Hr</t>
@@ -67,10 +70,7 @@
 Class,  Objects declaration, Methods, Constructors and Destructors(Garbage Collections - Memory management), Passing parameters to methods(By value &amp; By reference), Polymorphism  - Method Overloading, Constructor Overloading, static keywords, var args, static import.</t>
   </si>
   <si>
-    <t xml:space="preserve">19th July 20th July</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/2+1/2</t>
+    <t xml:space="preserve">21th July 22th July</t>
   </si>
   <si>
     <t xml:space="preserve">Inheritance, Overloading, Overriding</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">The concept of inheritance, conversion and casting in case of objects, override a method in subclass, covariant returns, super keyword, Method overriding(Dynamic method dispatch), final keyword</t>
   </si>
   <si>
-    <t xml:space="preserve">21th July 22th July</t>
+    <t xml:space="preserve">23rd July-24th july</t>
   </si>
   <si>
     <t xml:space="preserve">Abstract class, Interface, Inner classes</t>
@@ -88,13 +88,58 @@
     <t xml:space="preserve">Abstract keywrod, Definition, implementation of an interface, using interface, interface and multiple inheritance, interface to share constants, importance of setting standards, marker interface Types of inner classes, Static and non-static inner classes, local and anonymous inner classes, solid principles introduction </t>
   </si>
   <si>
-    <t xml:space="preserve">23rd July-24th july</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1+1/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12Hr</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">24</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> July +26</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> July</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">String, Exception handling, IO</t>
@@ -103,7 +148,7 @@
     <t xml:space="preserve">Object class, String class, StringBuffer, StringBuilder, Wrapper classes,primitive wrapper classes, immutability, autoboxing, Math class,The concept of exception handling, try blocks, Exception class methods, throw and rethrow , finally keyword, user-defined exceptions.Input/Output ; Serialization</t>
   </si>
   <si>
-    <t xml:space="preserve">26th july-27th july</t>
+    <t xml:space="preserve">27th july-28th july</t>
   </si>
   <si>
     <t xml:space="preserve">Assessment &amp; Review 1: Review Rajeev + Nilesh Kumar + Vir Bharat</t>
@@ -144,7 +189,37 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">28th july -29th july</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">29th july -20</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> july</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Multithreading</t>
@@ -153,7 +228,37 @@
     <t xml:space="preserve">Multithreading, Introduction to Threads, creation for child threads, Thread methods, synchronization, inter-thread communication</t>
   </si>
   <si>
-    <t xml:space="preserve">30th July-31st July</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">31</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> July</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Coding practice, GOF design patterns</t>
@@ -162,37 +267,7 @@
     <t xml:space="preserve">Java coding convensions, coding practice, code refactoring, SOLID principle, Intrdoction to GOF design pattern some commonly used design pattern</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">31</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">st</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> July-2nd Aug</t>
-    </r>
+    <t xml:space="preserve">2nd-3rd  Aug</t>
   </si>
   <si>
     <t xml:space="preserve">Assessment &amp; Review 2: Review Rajeev + Nilesh Kumar + Vir Bharat</t>
@@ -205,7 +280,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">3rd Aug-4th Aug</t>
+    <t xml:space="preserve">4rd Aug-5th Aug</t>
   </si>
   <si>
     <t xml:space="preserve">JDBC</t>
@@ -216,7 +291,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">5th Aug-6th Aug</t>
+    <t xml:space="preserve">6th Aug-7th Aug</t>
   </si>
   <si>
     <t xml:space="preserve">Java 8 Introduction</t>
@@ -225,7 +300,7 @@
     <t xml:space="preserve">Java 8 enhancements,, functional interface,Lambda vs Annonymous inner class,  Streams, Collectors basics</t>
   </si>
   <si>
-    <t xml:space="preserve">7th Aug</t>
+    <t xml:space="preserve">7th Aug-9th Aug</t>
   </si>
   <si>
     <t xml:space="preserve">Java 8 strem details</t>
@@ -234,7 +309,7 @@
     <t xml:space="preserve">Steam processing, Good programming practice, best practice using streams, method reference, Case stduy and examples. Easy data Paeallelism, Default and static methods on interfaces</t>
   </si>
   <si>
-    <t xml:space="preserve">9th Aug</t>
+    <t xml:space="preserve">10th Aug</t>
   </si>
   <si>
     <t xml:space="preserve">4Hr</t>
@@ -276,7 +351,37 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">10th Aug</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Aug</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve"> Assessment &amp; Review 3: Review Rajeev + Nilesh Kumar + Vir Bharat</t>
@@ -297,7 +402,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">11</t>
+      <t xml:space="preserve">12</t>
     </r>
     <r>
       <rPr>
@@ -337,7 +442,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">12</t>
+      <t xml:space="preserve">13</t>
     </r>
     <r>
       <rPr>
@@ -376,7 +481,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">13</t>
+      <t xml:space="preserve">16</t>
     </r>
     <r>
       <rPr>
@@ -415,7 +520,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">16</t>
+      <t xml:space="preserve">17</t>
     </r>
     <r>
       <rPr>
@@ -454,7 +559,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">17</t>
+      <t xml:space="preserve">18</t>
     </r>
     <r>
       <rPr>
@@ -496,7 +601,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">18</t>
+      <t xml:space="preserve">19</t>
     </r>
     <r>
       <rPr>
@@ -536,7 +641,7 @@
     <t xml:space="preserve">Hibernate Mapping:one to one, one to many, many to many etc, bidrectional, cascading,Hibernate HQL, criteria quaries, N+1 problem and solution,  Hibernate inheritance mapping and strategies</t>
   </si>
   <si>
-    <t xml:space="preserve">20th </t>
+    <t xml:space="preserve">20th Aug</t>
   </si>
   <si>
     <t xml:space="preserve">Hibernate performance ,Jooq</t>
@@ -774,12 +879,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -830,6 +936,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -842,20 +956,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1005,7 +1105,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1031,6 +1131,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1058,6 +1162,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1066,11 +1174,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1086,12 +1190,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1110,24 +1210,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1150,7 +1246,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1270,19 +1366,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="86.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="16.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="4" width="8.57"/>
@@ -1295,312 +1391,312 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="27.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+    <row r="3" customFormat="false" ht="31.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="C3" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="41.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="G3" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="66.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="n">
         <f aca="false">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="10" t="n">
+      <c r="B4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="G4" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="11" t="n">
         <f aca="false">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="n">
+      <c r="G5" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="73.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="n">
         <f aca="false">A5+1</f>
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>23</v>
+      <c r="F6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="66.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="n">
+      <c r="A7" s="17" t="n">
         <f aca="false">A6+1</f>
         <v>5</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="F7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="19"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="92.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
+      <c r="A9" s="17" t="n">
         <f aca="false">A7+1</f>
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="16" t="n">
-        <v>6</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="G9" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
+      <c r="A10" s="17" t="n">
         <f aca="false">A9+1</f>
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="16" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="F10" s="14" t="n">
+        <v>44228</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="79.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="C11" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="E11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="79.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="G11" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" customFormat="false" ht="68" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="C13" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="68" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="G13" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="84.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="C14" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="13" t="s">
+      <c r="E14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="84.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="G14" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="C15" s="22" t="n">
         <v>11</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="22" t="n">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>11</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1608,22 +1704,22 @@
         <v>12</v>
       </c>
       <c r="B16" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="22" t="n">
-        <v>12</v>
-      </c>
-      <c r="D16" s="23" t="s">
+      <c r="F16" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="24" t="s">
         <v>48</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1631,79 +1727,79 @@
         <v>13</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="22" t="n">
         <v>13</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="F17" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18" t="s">
-        <v>54</v>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="E18" s="18"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="19"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="43.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
         <v>14</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="22" t="n">
         <v>14</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="F19" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="n">
+      <c r="A20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="22" t="n">
         <v>15</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="F20" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="72.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1711,22 +1807,22 @@
         <v>16</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="22" t="n">
         <v>16</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="F21" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1734,20 +1830,20 @@
         <v>17</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="22" t="n">
         <v>17</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="77.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1755,79 +1851,79 @@
         <v>18</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="22" t="n">
         <v>18</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="F23" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="36.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18" t="s">
-        <v>70</v>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="E24" s="18"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="83.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="10" t="n">
-        <v>19</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="F25" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="42.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="42.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="n">
-        <v>20</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>74</v>
       </c>
       <c r="C26" s="22" t="n">
         <v>20</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="F26" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="30.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1835,22 +1931,22 @@
         <v>20</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="22" t="n">
         <v>21</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="F27" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="27.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1858,56 +1954,56 @@
         <v>21</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="22" t="n">
         <v>22</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="F28" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="22"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18" t="s">
-        <v>83</v>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="E29" s="18"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="19"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="46.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="27" t="n">
+        <v>23</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="C30" s="28" t="n">
-        <v>23</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>86</v>
       </c>
       <c r="F30" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="42.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1915,22 +2011,22 @@
         <v>24</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C31" s="22" t="n">
         <v>24</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="F31" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="47.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1938,22 +2034,22 @@
         <v>25</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" s="22" t="n">
         <v>25</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="F32" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1961,22 +2057,22 @@
         <v>26</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" s="22" t="n">
         <v>26</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="F33" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="49.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1984,22 +2080,22 @@
         <v>27</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="22" t="n">
         <v>27</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="F34" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="46.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2007,79 +2103,79 @@
         <v>28</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C35" s="22" t="n">
         <v>28</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="F35" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="60.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="94.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="n">
         <v>29</v>
       </c>
       <c r="B36" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="E36" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>105</v>
       </c>
       <c r="F36" s="22" t="n">
         <v>4</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="18" t="s">
-        <v>83</v>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="E37" s="18"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="19"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="87.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="n">
         <v>30</v>
       </c>
       <c r="B38" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="E38" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>110</v>
       </c>
       <c r="F38" s="22" t="n">
         <v>2</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="80.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2087,89 +2183,77 @@
         <v>34</v>
       </c>
       <c r="B39" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="E39" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>115</v>
       </c>
       <c r="F39" s="22" t="n">
         <v>2</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="40.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="E40" s="22" t="s">
         <v>117</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>119</v>
       </c>
       <c r="F40" s="22" t="n">
         <v>4</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="22"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="18" t="s">
-        <v>120</v>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="E41" s="18"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="19"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="24.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="22"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="G42" s="33" t="s">
-        <v>122</v>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="34"/>
+      <c r="A43" s="33"/>
     </row>
     <row r="44" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="35"/>
-    </row>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A44" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -2191,8 +2275,8 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2205,98 +2289,98 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">

</xml_diff>